<commit_message>
fixed windows decode issue
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -390,13 +390,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK8"/>
+  <dimension ref="A1:BK4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="15.85546875" bestFit="1" customWidth="1" min="4" max="4"/>
     <col width="14.42578125" customWidth="1" min="5" max="5"/>
@@ -448,7 +448,7 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Team 2 (Winner)</t>
+          <t>Team 2 (Loser)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -750,7 +750,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Splat Zones</t>
+          <t>templates/gamemodes\Splat Zones</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tower Control</t>
+          <t>templates/gamemodes\Tower Control</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Tower Control</t>
+          <t>templates/gamemodes\Tower Control</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="BE4" t="inlineStr">
         <is>
-          <t>Saffy#1132</t>
+          <t>ninety⏜*#2236</t>
         </is>
       </c>
       <c r="BF4" t="inlineStr">
@@ -1685,1274 +1685,6 @@
       <c r="BK4" t="inlineStr">
         <is>
           <t>1102</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Tower Control</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>daybreak</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Nightfall</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>LG|Bml#2702</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Clash Blaster</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>247</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>LG|Berny#2523</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Heavy Splatling</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>464</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>LG|Яηoodlε#2427</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>539</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>LG|JBYoshi#7013</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>507</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t>drey#7410</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>Heavy Splatling</t>
-        </is>
-      </c>
-      <c r="AL5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AN5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AO5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AP5" t="inlineStr">
-        <is>
-          <t>469</t>
-        </is>
-      </c>
-      <c r="AQ5" t="inlineStr">
-        <is>
-          <t>salty#8801</t>
-        </is>
-      </c>
-      <c r="AR5" t="inlineStr">
-        <is>
-          <t>Dark Tetra Dualies</t>
-        </is>
-      </c>
-      <c r="AS5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AT5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AU5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AV5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AW5" t="inlineStr">
-        <is>
-          <t>293</t>
-        </is>
-      </c>
-      <c r="AX5" t="inlineStr">
-        <is>
-          <t>galaxy☆#1325</t>
-        </is>
-      </c>
-      <c r="AY5" t="inlineStr">
-        <is>
-          <t>Flingza Roller</t>
-        </is>
-      </c>
-      <c r="AZ5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BA5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BB5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="BC5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BD5" t="inlineStr">
-        <is>
-          <t>534</t>
-        </is>
-      </c>
-      <c r="BE5" t="inlineStr">
-        <is>
-          <t>nax#1874</t>
-        </is>
-      </c>
-      <c r="BF5" t="inlineStr">
-        <is>
-          <t>Splash-o-matic Neo</t>
-        </is>
-      </c>
-      <c r="BG5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BH5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BI5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="BJ5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BK5" t="inlineStr">
-        <is>
-          <t>434</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Rainmaker</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>daybreak</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Nightfall</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>LG|Яηoodlε#2427</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>1607</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>LG|Berny#2523</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>Heavy Splatling</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>1378</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>LG|Bml#2702</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>Clash Blaster</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>839</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>LG|JBYoshi#7013</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>1331</t>
-        </is>
-      </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>LG|Salami#3369</t>
-        </is>
-      </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>.52 Gal</t>
-        </is>
-      </c>
-      <c r="AL6" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="AM6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AN6" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AO6" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AP6" t="inlineStr">
-        <is>
-          <t>1452</t>
-        </is>
-      </c>
-      <c r="AQ6" t="inlineStr">
-        <is>
-          <t>drey#7410</t>
-        </is>
-      </c>
-      <c r="AR6" t="inlineStr">
-        <is>
-          <t>Tri-Stringer</t>
-        </is>
-      </c>
-      <c r="AS6" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="AT6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AU6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AV6" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AW6" t="inlineStr">
-        <is>
-          <t>1310</t>
-        </is>
-      </c>
-      <c r="AX6" t="inlineStr">
-        <is>
-          <t>nax#1874</t>
-        </is>
-      </c>
-      <c r="AY6" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="AZ6" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="BA6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BB6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="BC6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="BD6" t="inlineStr">
-        <is>
-          <t>1330</t>
-        </is>
-      </c>
-      <c r="BE6" t="inlineStr">
-        <is>
-          <t>galaxy☆#1325</t>
-        </is>
-      </c>
-      <c r="BF6" t="inlineStr">
-        <is>
-          <t>Octobrush</t>
-        </is>
-      </c>
-      <c r="BG6" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="BH6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="BI6" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="BJ6" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="BK6" t="inlineStr">
-        <is>
-          <t>992</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Clam Blitz</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>daybreak</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Barracuda </t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>LG|Bml#2702</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Clash Blaster Neo</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>1102</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>LG|Berny#2523</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>Heavy Splatling</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>1467</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>LG|Яηoodlε#2427</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>1617</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>LG|nico!!#1146</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>Splat Roller</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>1287</t>
-        </is>
-      </c>
-      <c r="AJ7" t="inlineStr">
-        <is>
-          <t>Jp#4525</t>
-        </is>
-      </c>
-      <c r="AK7" t="inlineStr">
-        <is>
-          <t>Splat Roller</t>
-        </is>
-      </c>
-      <c r="AL7" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AM7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AN7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AO7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AP7" t="inlineStr">
-        <is>
-          <t>1143</t>
-        </is>
-      </c>
-      <c r="AQ7" t="inlineStr">
-        <is>
-          <t>Gummie#1813</t>
-        </is>
-      </c>
-      <c r="AR7" t="inlineStr">
-        <is>
-          <t>Splash-o-matic</t>
-        </is>
-      </c>
-      <c r="AS7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AT7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AU7" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AV7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AW7" t="inlineStr">
-        <is>
-          <t>1689</t>
-        </is>
-      </c>
-      <c r="AX7" t="inlineStr">
-        <is>
-          <t>Bagel#1138</t>
-        </is>
-      </c>
-      <c r="AY7" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="AZ7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BA7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BB7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BC7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BD7" t="inlineStr">
-        <is>
-          <t>1577</t>
-        </is>
-      </c>
-      <c r="BE7" t="inlineStr">
-        <is>
-          <t>TravelerCJ#1618</t>
-        </is>
-      </c>
-      <c r="BF7" t="inlineStr">
-        <is>
-          <t>Splatana Wiper</t>
-        </is>
-      </c>
-      <c r="BG7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BH7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BI7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BJ7" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BK7" t="inlineStr">
-        <is>
-          <t>1145</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Clam Blitz</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>daybreak</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Barracuda </t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>LG|Bml#2702</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Clash Blaster Neo</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>1102</t>
-        </is>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>LG|Berny#2523</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>Heavy Splatling</t>
-        </is>
-      </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>1467</t>
-        </is>
-      </c>
-      <c r="V8" t="inlineStr">
-        <is>
-          <t>LG|Яηoodlε#2427</t>
-        </is>
-      </c>
-      <c r="W8" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AB8" t="inlineStr">
-        <is>
-          <t>1617</t>
-        </is>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>LG|nico!!#1146</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>Splat Roller</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AG8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AH8" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AI8" t="inlineStr">
-        <is>
-          <t>1287</t>
-        </is>
-      </c>
-      <c r="AJ8" t="inlineStr">
-        <is>
-          <t>Jp#4525</t>
-        </is>
-      </c>
-      <c r="AK8" t="inlineStr">
-        <is>
-          <t>Splat Roller</t>
-        </is>
-      </c>
-      <c r="AL8" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AM8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AN8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AO8" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AP8" t="inlineStr">
-        <is>
-          <t>1143</t>
-        </is>
-      </c>
-      <c r="AQ8" t="inlineStr">
-        <is>
-          <t>Gummie#1813</t>
-        </is>
-      </c>
-      <c r="AR8" t="inlineStr">
-        <is>
-          <t>Splash-o-matic</t>
-        </is>
-      </c>
-      <c r="AS8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AT8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AU8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AV8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AW8" t="inlineStr">
-        <is>
-          <t>1689</t>
-        </is>
-      </c>
-      <c r="AX8" t="inlineStr">
-        <is>
-          <t>Bagel#1138</t>
-        </is>
-      </c>
-      <c r="AY8" t="inlineStr">
-        <is>
-          <t>Tentatek Splattershot</t>
-        </is>
-      </c>
-      <c r="AZ8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BA8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BB8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BC8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BD8" t="inlineStr">
-        <is>
-          <t>1577</t>
-        </is>
-      </c>
-      <c r="BE8" t="inlineStr">
-        <is>
-          <t>TravelerCJ#1618</t>
-        </is>
-      </c>
-      <c r="BF8" t="inlineStr">
-        <is>
-          <t>Splatana Wiper</t>
-        </is>
-      </c>
-      <c r="BG8" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BH8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BI8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BJ8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BK8" t="inlineStr">
-        <is>
-          <t>1145</t>
         </is>
       </c>
     </row>

</xml_diff>